<commit_message>
diagrama de grant actualizado
</commit_message>
<xml_diff>
--- a/diagrama de gantt.xlsx
+++ b/diagrama de gantt.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Horarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remoto\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAC8BAB0-C7BC-4ABA-B60A-FDEDFD0395D1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,13 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
-  <si>
-    <t>PROYECTO: Cargas Academicas UDEO</t>
-  </si>
-  <si>
-    <t>LIDER DE PROYECTO: Fabian Vazquez Dominguez</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>DIAGRAMA DE GANTT</t>
   </si>
@@ -47,21 +42,6 @@
     <t>SEMANA 5</t>
   </si>
   <si>
-    <t>del 11 al 20 de enero</t>
-  </si>
-  <si>
-    <t>del 21 al 03 de febrero</t>
-  </si>
-  <si>
-    <t>del 04 al 17 de febrero</t>
-  </si>
-  <si>
-    <t>del 18 al 03 de marzo</t>
-  </si>
-  <si>
-    <t>del 04 al 17 de marzo</t>
-  </si>
-  <si>
     <t>ACTIVIDADES</t>
   </si>
   <si>
@@ -98,31 +78,88 @@
     <t>Marcos Navarro</t>
   </si>
   <si>
-    <t>Antonio Cortez</t>
-  </si>
-  <si>
     <t>Tester del programa y creación de documentación del testeo</t>
   </si>
   <si>
     <t>Diseño de interfaces y verificación de la integridad de los datos</t>
   </si>
   <si>
-    <t>Desarrollador y corrección de errores en testeo</t>
-  </si>
-  <si>
-    <t>Desarrollador y correccion de errores en testeo</t>
-  </si>
-  <si>
     <t>Desarrollo del reporteador</t>
   </si>
   <si>
-    <t>Diseño de interfaces</t>
+    <t>del 5 al 09 de noviembre</t>
+  </si>
+  <si>
+    <t>del 12 al 16 de noviembre</t>
+  </si>
+  <si>
+    <t>Correccion de la integridad de los datos</t>
+  </si>
+  <si>
+    <t>PROYECTO: Cargas Academicas UADEO</t>
+  </si>
+  <si>
+    <t>Testeo</t>
+  </si>
+  <si>
+    <t>Documentacion</t>
+  </si>
+  <si>
+    <t>documentacion</t>
+  </si>
+  <si>
+    <t>testeo</t>
+  </si>
+  <si>
+    <t>diseño de interfaces</t>
+  </si>
+  <si>
+    <t>verificacion de datos</t>
+  </si>
+  <si>
+    <t>diseño de interfaz</t>
+  </si>
+  <si>
+    <t>correccion de errores</t>
+  </si>
+  <si>
+    <t>correccion de integridad de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diseño de interfaces </t>
+  </si>
+  <si>
+    <t>correccion de errores en testeo</t>
+  </si>
+  <si>
+    <t>Diseño de interfaz</t>
+  </si>
+  <si>
+    <t>Testeo del reporteador</t>
+  </si>
+  <si>
+    <t>Correccion de errores del reporteador</t>
+  </si>
+  <si>
+    <t>Desarrollo y testeo del reporteador</t>
+  </si>
+  <si>
+    <t>del 19 al 23 de noviembre</t>
+  </si>
+  <si>
+    <t>del 26 al 30 de noviembre</t>
+  </si>
+  <si>
+    <t>del 29 de octubre al 2 de noviembre</t>
+  </si>
+  <si>
+    <t>Lider del proyecto: Jose Rene Armenta Polanco</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -202,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -273,10 +310,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -285,6 +328,17 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -294,42 +348,62 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -360,16 +434,41 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,6 +562,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -498,6 +614,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -673,337 +806,415 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="7" max="7" width="37.42578125" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="31.85546875" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" customWidth="1"/>
+    <col min="13" max="13" width="34.7109375" customWidth="1"/>
+    <col min="15" max="15" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="C1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+      <c r="H4" s="20"/>
+      <c r="I4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="16" t="s">
+      <c r="J4" s="20"/>
+      <c r="K4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16" t="s">
+      <c r="L4" s="20"/>
+      <c r="M4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16" t="s">
+      <c r="N4" s="20"/>
+      <c r="O4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16" t="s">
+      <c r="P4" s="20"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="20"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="16"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="16" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16" t="s">
+      <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16" t="s">
+      <c r="I7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="31"/>
+      <c r="I8" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="31"/>
+      <c r="M8" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="31"/>
+      <c r="O8" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="31"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="32"/>
+      <c r="I9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="32"/>
+      <c r="K9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="32"/>
+      <c r="M9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="32"/>
+      <c r="O9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" s="32"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="32"/>
+      <c r="K10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="32"/>
+      <c r="M10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="32"/>
+      <c r="O10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="32"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="32"/>
+      <c r="I11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="32"/>
+      <c r="K11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="32"/>
+      <c r="M11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="32"/>
+      <c r="O11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P11" s="32"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="32"/>
+      <c r="I12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="32"/>
+      <c r="K12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="32"/>
+      <c r="M12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="32"/>
+      <c r="O12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" s="32"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="24"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="24"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G15" s="36"/>
+      <c r="M15" s="28"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="29"/>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="16"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E16" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G19" s="6"/>
+      <c r="G19" s="33"/>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G21" s="33"/>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G22" s="24"/>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="H27" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
+    <mergeCell ref="O4:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="K4:L5"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="G4:H5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M4:N5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F6"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="B8:C8"/>
@@ -1017,21 +1228,7 @@
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F6"/>
-    <mergeCell ref="O4:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="K4:L5"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="G4:H5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M4:N5"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1039,7 +1236,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1051,7 +1248,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>